<commit_message>
Toevoeging referentieregio's + aggregatietabel gemeente_gewest
</commit_message>
<xml_diff>
--- a/data_voor_swing/aggregatietabellen/vervoerregio_gewest.xlsx
+++ b/data_voor_swing/aggregatietabellen/vervoerregio_gewest.xlsx
@@ -382,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -401,122 +401,176 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="0" outlineLevel="0">
-      <c r="A2" s="23">
-        <v>1</v>
+      <c r="A2" t="n">
+        <v/>
       </c>
       <c r="B2" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="0" outlineLevel="0">
-      <c r="A3" s="23">
-        <v>2</v>
+      <c r="A3" t="n">
+        <v/>
       </c>
       <c r="B3" s="23">
-        <v>2000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="0" outlineLevel="0">
-      <c r="A4" s="23">
-        <v>3</v>
+      <c r="A4" t="n">
+        <v/>
       </c>
       <c r="B4" s="23">
-        <v>2000</v>
+        <v>99999</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="0" outlineLevel="0">
-      <c r="A5" s="23">
-        <v>4</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B5" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="0" outlineLevel="0">
-      <c r="A6" s="23">
-        <v>5</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="B6" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="0" outlineLevel="0">
-      <c r="A7" s="23">
-        <v>6</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="B7" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="0" outlineLevel="0">
-      <c r="A8" s="23">
-        <v>7</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="B8" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="0" outlineLevel="0">
-      <c r="A9" s="23">
-        <v>8</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
       <c r="B9" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="0" outlineLevel="0">
-      <c r="A10" s="23">
-        <v>9</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
       <c r="B10" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="0" outlineLevel="0">
-      <c r="A11" s="23">
-        <v>10</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
       <c r="B11" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="0" outlineLevel="0">
-      <c r="A12" s="23">
-        <v>11</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B12" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="0" outlineLevel="0">
-      <c r="A13" s="23">
-        <v>12</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="B13" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="0" outlineLevel="0">
-      <c r="A14" s="23">
-        <v>13</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="B14" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="0" outlineLevel="0">
-      <c r="A15" s="23">
-        <v>14</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B15" s="23">
         <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="0" outlineLevel="0">
-      <c r="A16" s="23">
-        <v>15</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B16" s="23">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="0" outlineLevel="0">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B17" s="23">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="0" outlineLevel="0">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B18" s="23">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="0" outlineLevel="0">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B19" s="23">
         <v>2000</v>
       </c>
     </row>

</xml_diff>